<commit_message>
Módulo 08 - Fŕomulas intermediárias soma.se(s)/Média.se(s)
</commit_message>
<xml_diff>
--- a/módulo 08/aula-media-se.xlsx
+++ b/módulo 08/aula-media-se.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\10 Fórmulas avançadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 08\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BaseDados" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -217,12 +217,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -234,7 +234,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -274,34 +274,34 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -311,7 +311,7 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -46704,8 +46704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46786,8 +46786,14 @@
         <f>SUMIF(TbVendas[LOJA],B7,TbVendas[VALOR])</f>
         <v>77069</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="27"/>
+      <c r="F7" s="21">
+        <f>AVERAGEIF(TbVendas[LOJA],B7,TbVendas[VOLUME])</f>
+        <v>15.237903225806452</v>
+      </c>
+      <c r="G7" s="27">
+        <f>AVERAGEIF(TbVendas[LOJA],B7,TbVendas[VALOR])</f>
+        <v>155.38104838709677</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -46801,8 +46807,14 @@
         <f>SUMIF(TbVendas[LOJA],B8,TbVendas[VALOR])</f>
         <v>84906</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="28"/>
+      <c r="F8" s="23">
+        <f>AVERAGEIF(TbVendas[LOJA],B8,TbVendas[VOLUME])</f>
+        <v>16.272030651340994</v>
+      </c>
+      <c r="G8" s="28">
+        <f>AVERAGEIF(TbVendas[LOJA],B8,TbVendas[VALOR])</f>
+        <v>162.65517241379311</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
@@ -46816,8 +46828,14 @@
         <f>SUMIF(TbVendas[LOJA],B9,TbVendas[VALOR])</f>
         <v>81247</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="23">
+        <f>AVERAGEIF(TbVendas[LOJA],B9,TbVendas[VOLUME])</f>
+        <v>15.673999999999999</v>
+      </c>
+      <c r="G9" s="28">
+        <f>AVERAGEIF(TbVendas[LOJA],B9,TbVendas[VALOR])</f>
+        <v>162.494</v>
+      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
@@ -46831,8 +46849,14 @@
         <f>SUMIF(TbVendas[LOJA],B10,TbVendas[VALOR])</f>
         <v>77743</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="29"/>
+      <c r="F10" s="25">
+        <f>AVERAGEIF(TbVendas[LOJA],B10,TbVendas[VOLUME])</f>
+        <v>15.591286307053942</v>
+      </c>
+      <c r="G10" s="29">
+        <f>AVERAGEIF(TbVendas[LOJA],B10,TbVendas[VALOR])</f>
+        <v>161.29253112033194</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -46844,8 +46868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Módulo 08 - Fŕomulas intermediárias soma.se(s)/Média.se(ses)
</commit_message>
<xml_diff>
--- a/módulo 08/aula-media-se.xlsx
+++ b/módulo 08/aula-media-se.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6180" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BaseDados" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,9 @@
   </sheetPr>
   <dimension ref="A1:H2001"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -46704,8 +46706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46868,8 +46870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46937,6 +46939,10 @@
       <c r="G6" s="17" t="s">
         <v>4</v>
       </c>
+      <c r="L6" s="12">
+        <f>AVERAGEIFS(TbVendas[VALOR],TbVendas[LOJA],B8,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
+        <v>166.55072463768116</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -46944,14 +46950,20 @@
       </c>
       <c r="C7" s="21">
         <f>SUMIFS(TbVendas[VOLUME],TbVendas[LOJA],B7,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>1007</v>
+        <v>850</v>
       </c>
       <c r="D7" s="22">
         <f>SUMIFS(TbVendas[VALOR],TbVendas[LOJA],B7,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>10082</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="27"/>
+        <v>9213</v>
+      </c>
+      <c r="F7" s="21">
+        <f>AVERAGEIFS(TbVendas[VOLUME],TbVendas[LOJA],B7,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
+        <v>14.40677966101695</v>
+      </c>
+      <c r="G7" s="27">
+        <f>AVERAGEIFS(TbVendas[VALOR],TbVendas[LOJA],B7,TbVendas[CATEGORIA],$C$12, TbVendas[GÊNERO],$C$13)</f>
+        <v>156.15254237288136</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -46959,14 +46971,20 @@
       </c>
       <c r="C8" s="23">
         <f>SUMIFS(TbVendas[VOLUME],TbVendas[LOJA],B8,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>1345</v>
+        <v>1150</v>
       </c>
       <c r="D8" s="24">
         <f>SUMIFS(TbVendas[VALOR],TbVendas[LOJA],B8,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>13101</v>
-      </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="28"/>
+        <v>11492</v>
+      </c>
+      <c r="F8" s="23">
+        <f>AVERAGEIFS(TbVendas[VOLUME],TbVendas[LOJA],B8,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="G8" s="28">
+        <f>AVERAGEIFS(TbVendas[VALOR],TbVendas[LOJA],B8,TbVendas[CATEGORIA],$C$12, TbVendas[GÊNERO],$C$13)</f>
+        <v>166.55072463768116</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
@@ -46974,14 +46992,20 @@
       </c>
       <c r="C9" s="23">
         <f>SUMIFS(TbVendas[VOLUME],TbVendas[LOJA],B9,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>951</v>
+        <v>938</v>
       </c>
       <c r="D9" s="24">
         <f>SUMIFS(TbVendas[VALOR],TbVendas[LOJA],B9,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>11220</v>
-      </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="28"/>
+        <v>9129</v>
+      </c>
+      <c r="F9" s="23">
+        <f>AVERAGEIFS(TbVendas[VOLUME],TbVendas[LOJA],B9,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
+        <v>16.75</v>
+      </c>
+      <c r="G9" s="28">
+        <f>AVERAGEIFS(TbVendas[VALOR],TbVendas[LOJA],B9,TbVendas[CATEGORIA],$C$12, TbVendas[GÊNERO],$C$13)</f>
+        <v>163.01785714285714</v>
+      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
@@ -46989,14 +47013,20 @@
       </c>
       <c r="C10" s="25">
         <f>SUMIFS(TbVendas[VOLUME],TbVendas[LOJA],B10,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>1239</v>
+        <v>681</v>
       </c>
       <c r="D10" s="26">
         <f>SUMIFS(TbVendas[VALOR],TbVendas[LOJA],B10,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
-        <v>12231</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="29"/>
+        <v>5049</v>
+      </c>
+      <c r="F10" s="25">
+        <f>AVERAGEIFS(TbVendas[VOLUME],TbVendas[LOJA],B10,TbVendas[CATEGORIA],$C$12,TbVendas[GÊNERO],$C$13)</f>
+        <v>16.609756097560975</v>
+      </c>
+      <c r="G10" s="29">
+        <f>AVERAGEIFS(TbVendas[VALOR],TbVendas[LOJA],B10,TbVendas[CATEGORIA],$C$12, TbVendas[GÊNERO],$C$13)</f>
+        <v>123.14634146341463</v>
+      </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
@@ -47011,7 +47041,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -47036,5 +47066,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Módulo 09 - Projeto estoque part 05
</commit_message>
<xml_diff>
--- a/módulo 08/aula-media-se.xlsx
+++ b/módulo 08/aula-media-se.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8037" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8041" uniqueCount="30">
   <si>
     <t>DATA</t>
   </si>
@@ -108,6 +108,18 @@
   <si>
     <t>MÉDIAS POR LOJA, CATEGORIA E GÊNERO</t>
   </si>
+  <si>
+    <t xml:space="preserve">MédiaSe e MédiaSes </t>
+  </si>
+  <si>
+    <t>São similares ao somase e ao somaSes onde o média ao invés de tirar a soma</t>
+  </si>
+  <si>
+    <t>tira a média: o médiase pega o intervalo onde aerá tirada a média ao final da expressão</t>
+  </si>
+  <si>
+    <t>enquanto o médiases pega o valor da média no primeiro atributo da expressão</t>
+  </si>
 </sst>
 </file>
 
@@ -118,7 +130,7 @@
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +164,14 @@
       <b/>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -303,6 +323,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -46704,10 +46733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46860,6 +46889,33 @@
         <v>161.29253112033194</v>
       </c>
     </row>
+    <row r="14" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="34"/>
+      <c r="C15"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -46868,10 +46924,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47044,17 +47100,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C15"/>
-    </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="33">
+        <f>AVERAGEIFS(TbVendas[VOLUME],TbVendas[LOJA],B7,TbVendas[CATEGORIA],C12,TbVendas[GÊNERO],C13)</f>
+        <v>14.40677966101695</v>
+      </c>
       <c r="C17"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
+        <f>AVERAGEIFS(TbVendas[VALOR],TbVendas[LOJA],B7,TbVendas[CATEGORIA],C12,TbVendas[GÊNERO],C13)</f>
+        <v>156.15254237288136</v>
+      </c>
       <c r="C18"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>